<commit_message>
added function that creates requisition prep sheets
</commit_message>
<xml_diff>
--- a/prep_and_checklists/Adrianne Graves Baby Shower/Adrianne Graves Baby Shower_2025-04-12_0.xlsx
+++ b/prep_and_checklists/Adrianne Graves Baby Shower/Adrianne Graves Baby Shower_2025-04-12_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/prep_and_checklists/Adrianne Graves Baby Shower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00671B68-9EB6-794F-B2D3-D3751D711A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572F1A0B-B48C-E944-A8FA-1DD8377A4EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prep_sheet" sheetId="1" r:id="rId1"/>
@@ -243,7 +243,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +277,24 @@
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -321,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -331,6 +349,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,10 +658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A5" sqref="A5:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -655,249 +683,265 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="14" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="21" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="29" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="35" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="6" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <pageSetup scale="79" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1071,5 +1115,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>